<commit_message>
validation error is added
</commit_message>
<xml_diff>
--- a/wait/dst_working/جروب B - استمارة تقييم مهرجان 2020 - المستوى الرابع.xlsx
+++ b/wait/dst_working/جروب B - استمارة تقييم مهرجان 2020 - المستوى الرابع.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4476" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="4476" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="ك الملاك رافائيل بالمعادى" sheetId="1" r:id="rId1"/>
@@ -1087,7 +1087,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2694,18 +2694,18 @@
       <c r="D70" s="25"/>
       <c r="E70" s="25"/>
       <c r="F70" s="9">
-        <f t="shared" ref="F70:F101" si="6">SUM(C70:E70)*$F$2</f>
+        <f t="shared" ref="F70:F77" si="6">SUM(C70:E70)*$F$2</f>
         <v>0</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="16">
-        <f t="shared" ref="J70:J101" si="7">SUM(G70:I70)*$J$2</f>
+        <f t="shared" ref="J70:J77" si="7">SUM(G70:I70)*$J$2</f>
         <v>0</v>
       </c>
       <c r="K70" s="17">
-        <f t="shared" ref="K70:K101" si="8">J70+F70</f>
+        <f t="shared" ref="K70:K77" si="8">J70+F70</f>
         <v>0</v>
       </c>
     </row>
@@ -5083,18 +5083,18 @@
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="9">
-        <f t="shared" ref="F70:F101" si="6">SUM(C70:E70)*$F$2</f>
+        <f t="shared" ref="F70:F77" si="6">SUM(C70:E70)*$F$2</f>
         <v>0</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="16">
-        <f t="shared" ref="J70:J101" si="7">SUM(G70:I70)*$J$2</f>
+        <f t="shared" ref="J70:J77" si="7">SUM(G70:I70)*$J$2</f>
         <v>0</v>
       </c>
       <c r="K70" s="17">
-        <f t="shared" ref="K70:K101" si="8">J70+F70</f>
+        <f t="shared" ref="K70:K77" si="8">J70+F70</f>
         <v>0</v>
       </c>
     </row>
@@ -8010,18 +8010,18 @@
       <c r="D70" s="25"/>
       <c r="E70" s="25"/>
       <c r="F70" s="9">
-        <f t="shared" ref="F70:F101" si="6">SUM(C70:E70)*$F$2</f>
+        <f t="shared" ref="F70:F77" si="6">SUM(C70:E70)*$F$2</f>
         <v>0</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="16">
-        <f t="shared" ref="J70:J101" si="7">SUM(G70:I70)*$J$2</f>
+        <f t="shared" ref="J70:J77" si="7">SUM(G70:I70)*$J$2</f>
         <v>0</v>
       </c>
       <c r="K70" s="17">
-        <f t="shared" ref="K70:K101" si="8">J70+F70</f>
+        <f t="shared" ref="K70:K77" si="8">J70+F70</f>
         <v>0</v>
       </c>
     </row>
@@ -10564,18 +10564,18 @@
       <c r="D70" s="25"/>
       <c r="E70" s="25"/>
       <c r="F70" s="9">
-        <f t="shared" ref="F70:F101" si="6">SUM(C70:E70)*$F$2</f>
+        <f t="shared" ref="F70:F77" si="6">SUM(C70:E70)*$F$2</f>
         <v>0</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="16">
-        <f t="shared" ref="J70:J101" si="7">SUM(G70:I70)*$J$2</f>
+        <f t="shared" ref="J70:J77" si="7">SUM(G70:I70)*$J$2</f>
         <v>0</v>
       </c>
       <c r="K70" s="17">
-        <f t="shared" ref="K70:K101" si="8">J70+F70</f>
+        <f t="shared" ref="K70:K77" si="8">J70+F70</f>
         <v>0</v>
       </c>
     </row>
@@ -12953,18 +12953,18 @@
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="9">
-        <f t="shared" ref="F70:F101" si="6">SUM(C70:E70)*$F$2</f>
+        <f t="shared" ref="F70:F77" si="6">SUM(C70:E70)*$F$2</f>
         <v>0</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="16">
-        <f t="shared" ref="J70:J101" si="7">SUM(G70:I70)*$J$2</f>
+        <f t="shared" ref="J70:J77" si="7">SUM(G70:I70)*$J$2</f>
         <v>0</v>
       </c>
       <c r="K70" s="17">
-        <f t="shared" ref="K70:K101" si="8">J70+F70</f>
+        <f t="shared" ref="K70:K77" si="8">J70+F70</f>
         <v>0</v>
       </c>
     </row>
@@ -13764,8 +13764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K129"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="D3" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="B3" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -15404,18 +15404,18 @@
       <c r="D70" s="25"/>
       <c r="E70" s="25"/>
       <c r="F70" s="9">
-        <f t="shared" ref="F70:F101" si="6">SUM(C70:E70)*$F$2</f>
+        <f t="shared" ref="F70:F77" si="6">SUM(C70:E70)*$F$2</f>
         <v>0</v>
       </c>
       <c r="G70" s="3"/>
       <c r="H70" s="3"/>
       <c r="I70" s="3"/>
       <c r="J70" s="16">
-        <f t="shared" ref="J70:J101" si="7">SUM(G70:I70)*$J$2</f>
+        <f t="shared" ref="J70:J77" si="7">SUM(G70:I70)*$J$2</f>
         <v>0</v>
       </c>
       <c r="K70" s="17">
-        <f t="shared" ref="K70:K101" si="8">J70+F70</f>
+        <f t="shared" ref="K70:K77" si="8">J70+F70</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>